<commit_message>
add columns to data
</commit_message>
<xml_diff>
--- a/Data/cambodia_projects.xlsx
+++ b/Data/cambodia_projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmid_nat\Documents\giz_mapping\toy_dash_application\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC5643C-DE94-417C-838F-8E8DE2CAC141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5CF717-347E-44F9-A0F0-9990514795DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11580" yWindow="-15990" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{7AEC4126-3C7B-4D00-A9A3-6376038D8029}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7AEC4126-3C7B-4D00-A9A3-6376038D8029}"/>
   </bookViews>
   <sheets>
     <sheet name="cambodia_projects" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="95">
   <si>
     <t>project_id</t>
   </si>
@@ -314,6 +314,18 @@
   </si>
   <si>
     <t>As a farmer in Pursat Province, I have faced challenges in accessing quality agricultural inputs and technologies. However, thanks to the Productivity Enhancement Support project, my farming practices have been revolutionized. The subsidized certified seeds, fertilizer, and training provided have not only increased my crop yields but have also diversified my livelihood options. I've been able to experiment with new crops and techniques, leading to improved resilience against environmental fluctuations. This support has not only boosted my family's food security but has also enhanced our income opportunities. I'm incredibly grateful for the opportunities this project has provided</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>KHM</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>infrastructure</t>
   </si>
 </sst>
 </file>
@@ -679,20 +691,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CE4B7E-51F1-4C7C-A730-9198D98BB961}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,28 +713,34 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="170.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="170.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -729,28 +748,34 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>12.391061000000001</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>105.114631</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>14750000</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="180.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="180.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -758,24 +783,30 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>12.763653</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>105.04560499999999</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>10000000</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2115,7 +2146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EF6E02-44A4-44C7-8B59-944C64BAB2F8}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>